<commit_message>
Added another survey input.
</commit_message>
<xml_diff>
--- a/Survey_DB.xlsx
+++ b/Survey_DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="155">
   <si>
     <t>ID_fisher</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>Paquera</t>
+  </si>
+  <si>
+    <t>Paquera Tambor</t>
   </si>
 </sst>
 </file>
@@ -841,7 +844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -853,7 +856,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1484,6 +1487,9 @@
       <c r="D5" t="s">
         <v>153</v>
       </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Alex made test changes
</commit_message>
<xml_diff>
--- a/Survey_DB.xlsx
+++ b/Survey_DB.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Diana_Flores/Documents/nicoyafisheries.github.io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrasmith/Documents/GP_git/nicoyafisheries.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,8 @@
     <sheet name="Wagner" sheetId="1" r:id="rId1"/>
     <sheet name="Q9_Wagner" sheetId="2" r:id="rId2"/>
     <sheet name="Alex" sheetId="4" r:id="rId3"/>
-    <sheet name="Diana" sheetId="5" r:id="rId4"/>
+    <sheet name="Q9_Alex" sheetId="6" r:id="rId4"/>
+    <sheet name="Diana" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="162">
   <si>
     <t>ID_fisher</t>
   </si>
@@ -513,6 +514,9 @@
   </si>
   <si>
     <t>están</t>
+  </si>
+  <si>
+    <t>dear god</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1536,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1598,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF5"/>
+  <dimension ref="A1:CF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2202,6 +2206,14 @@
         <v>156</v>
       </c>
     </row>
+    <row r="6" spans="1:84" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="W2:AE2"/>
@@ -2212,9 +2224,75 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ALEX tests again again
</commit_message>
<xml_diff>
--- a/Survey_DB.xlsx
+++ b/Survey_DB.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacia Rivera\Desktop\GitHub\nicoyafisheries.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrasmith/Documents/GP_git/nicoyafisheries.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="500" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wagner" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="163">
   <si>
     <t>ID_fisher</t>
   </si>
@@ -520,12 +520,15 @@
   </si>
   <si>
     <t>dear god</t>
+  </si>
+  <si>
+    <t>kuysdlhzjgldf;slkhvai;l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -894,75 +897,75 @@
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" style="2"/>
-    <col min="12" max="12" width="7.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="2"/>
+    <col min="12" max="12" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="2.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="2.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="11" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="13.5" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="54" max="56" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="9" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="16.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="67" max="69" width="10.875" style="7"/>
-    <col min="70" max="72" width="10.875" style="5"/>
-    <col min="73" max="75" width="10.875" style="7"/>
-    <col min="76" max="78" width="10.875" style="5"/>
-    <col min="79" max="81" width="10.875" style="7"/>
-    <col min="82" max="84" width="10.875" style="5"/>
+    <col min="63" max="63" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="67" max="69" width="11" style="7"/>
+    <col min="70" max="72" width="11" style="5"/>
+    <col min="73" max="75" width="11" style="7"/>
+    <col min="76" max="78" width="11" style="5"/>
+    <col min="79" max="81" width="11" style="7"/>
+    <col min="82" max="84" width="11" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.25">
@@ -1545,9 +1548,9 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1614,7 +1617,7 @@
       <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="H1" s="2" t="s">
@@ -2230,13 +2233,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
@@ -2287,6 +2290,11 @@
       </c>
       <c r="G3" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2302,7 +2310,7 @@
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="H1" s="2" t="s">
@@ -2892,7 +2900,7 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -2919,7 +2927,7 @@
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
@@ -2985,7 +2993,7 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="H1" s="2" t="s">
@@ -3575,7 +3583,7 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -3598,11 +3606,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">

</xml_diff>

<commit_message>
added histogram of ages for corvina 2012
</commit_message>
<xml_diff>
--- a/Survey_DB.xlsx
+++ b/Survey_DB.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrasmith/Documents/GP_git/nicoyafisheries.github.io/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wagner" sheetId="1" r:id="rId1"/>
@@ -18,18 +23,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="178">
   <si>
     <t>ID_fisher</t>
   </si>
@@ -496,12 +501,6 @@
     <t>Marina Quiros</t>
   </si>
   <si>
-    <t xml:space="preserve">test </t>
-  </si>
-  <si>
-    <t>please work</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -514,13 +513,61 @@
     <t>están</t>
   </si>
   <si>
-    <t>dear god</t>
-  </si>
-  <si>
     <t>kuysdlhzjgldf;slkhvai;l</t>
   </si>
   <si>
     <t>Por Favor Dios, Ala y Budha</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>JH</t>
+  </si>
+  <si>
+    <t>Isla Venado</t>
+  </si>
+  <si>
+    <t>Asoc. Local Pescadores de Florida</t>
+  </si>
+  <si>
+    <t>Presidente</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Gillnet sizes : 3-3.5 for shrimp/6 for corvina</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>Hace 6 años eran mejores, gente respectaba y guara costa hacia su trabajo. Cambio y falta de recursos de guarda costa. Ademas narcotrafico</t>
+  </si>
+  <si>
+    <t>salario minimo</t>
+  </si>
+  <si>
+    <t>caos totalm no so respetana mucho/complicado organizar y coordinar tantos pescadores/much tiempo pescando con un arte especifico en sito especifico</t>
+  </si>
+  <si>
+    <t>seria bueno, idealmente en la zona 201 que es un puro criadero/al principio seria terrible y pescadores que estan dentro de esa zona. Problemas con las licencias que delimitan sitios de pesca/necesitaria reestructura de INCOPESCA y sus licensias</t>
+  </si>
+  <si>
+    <t>debe hacer mucha coordinacion/las islas se depoblanan/tiene que hacber ayuda y vigilancia muy buena</t>
+  </si>
+  <si>
+    <t>145 mil se podrian usar en control y vigilancia y que los pescadoeres ahorren y tengan guardado para los meses de veda/ seria bueno</t>
+  </si>
+  <si>
+    <t>no fuciona/hace 3 años vienen haciendo vedas diferenicadas y no funcionaban basado en conocimiento tradicional</t>
+  </si>
+  <si>
+    <t>conflicto grande de comunidades/no todos los asocidos pescan con cuerda o dentro del AMPR con esa arte de pesca/Muchos no-asociados pescan dentro</t>
   </si>
 </sst>
 </file>
@@ -550,7 +597,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,6 +613,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -608,6 +661,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,7 +937,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -890,12 +947,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
@@ -966,7 +1023,7 @@
     <col min="82" max="84" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1124,7 +1181,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1270,7 +1327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:84" s="8" customFormat="1">
+    <row r="3" spans="1:84" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -1510,7 +1567,7 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="5" spans="1:84">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -1527,12 +1584,12 @@
         <v>153</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:84">
+    <row r="6" spans="1:84" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1540,11 +1597,6 @@
     <mergeCell ref="W2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1556,12 +1608,12 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>63</v>
       </c>
@@ -1578,7 +1630,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1589,7 +1641,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1614,25 +1666,96 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF6"/>
+  <dimension ref="A1:CG4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BX4" sqref="BX4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="10" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="10" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="10" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="7" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="36.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:84">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1814,8 +1937,11 @@
       <c r="CF1" s="5" t="s">
         <v>138</v>
       </c>
+      <c r="CG1" s="5" t="s">
+        <v>167</v>
+      </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1980,7 +2106,7 @@
       </c>
       <c r="CF2" s="5"/>
     </row>
-    <row r="3" spans="1:84" s="8" customFormat="1">
+    <row r="3" spans="1:85" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -2220,20 +2346,259 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="5" spans="1:84">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:84">
-      <c r="A6" t="s">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>161</v>
       </c>
-      <c r="B6" t="s">
-        <v>156</v>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="14">
+        <v>42567</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>164</v>
+      </c>
+      <c r="L4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M4">
+        <v>15</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>166</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>600</v>
+      </c>
+      <c r="V4" t="s">
+        <v>166</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>6</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <f>AVERAGE(500, 1000)</f>
+        <v>750</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>12</v>
+      </c>
+      <c r="AU4">
+        <v>15</v>
+      </c>
+      <c r="AV4" s="16">
+        <f>AVERAGE(9,10,2)</f>
+        <v>7</v>
+      </c>
+      <c r="AW4" s="16">
+        <v>7</v>
+      </c>
+      <c r="AX4">
+        <f>AVERAGE(3000,4000)</f>
+        <v>3500</v>
+      </c>
+      <c r="AZ4">
+        <f>AVERAGE(300000,400000)</f>
+        <v>350000</v>
+      </c>
+      <c r="BA4">
+        <v>2</v>
+      </c>
+      <c r="BB4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BC4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD4">
+        <v>80000</v>
+      </c>
+      <c r="BE4" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="BF4">
+        <v>0.5</v>
+      </c>
+      <c r="BG4">
+        <v>0.5</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="BK4" s="17">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="17">
+        <v>1</v>
+      </c>
+      <c r="BM4" s="17">
+        <v>0</v>
+      </c>
+      <c r="BN4" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="BO4" s="17">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="17">
+        <v>1</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>172</v>
+      </c>
+      <c r="BR4">
+        <v>0</v>
+      </c>
+      <c r="BS4">
+        <v>1</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>176</v>
+      </c>
+      <c r="BU4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>1</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>177</v>
+      </c>
+      <c r="BX4">
+        <v>1</v>
+      </c>
+      <c r="BY4">
+        <v>1</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>173</v>
+      </c>
+      <c r="CA4">
+        <v>0</v>
+      </c>
+      <c r="CB4">
+        <v>1</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>174</v>
+      </c>
+      <c r="CD4">
+        <v>1</v>
+      </c>
+      <c r="CE4">
+        <v>0</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>175</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2241,11 +2606,6 @@
     <mergeCell ref="W2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2257,9 +2617,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>63</v>
       </c>
@@ -2276,7 +2636,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2287,7 +2647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -2310,18 +2670,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2333,9 +2688,9 @@
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:84">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
@@ -2518,7 +2873,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2683,7 +3038,7 @@
       </c>
       <c r="CF2" s="5"/>
     </row>
-    <row r="3" spans="1:84" s="8" customFormat="1">
+    <row r="3" spans="1:84" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -2923,15 +3278,15 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="5" spans="1:84">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
         <v>158</v>
-      </c>
-      <c r="B5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2939,11 +3294,6 @@
     <mergeCell ref="W2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2955,9 +3305,9 @@
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>63</v>
       </c>
@@ -2974,7 +3324,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2985,7 +3335,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -3010,11 +3360,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3026,9 +3371,9 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:84">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
@@ -3211,7 +3556,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -3376,7 +3721,7 @@
       </c>
       <c r="CF2" s="5"/>
     </row>
-    <row r="3" spans="1:84" s="8" customFormat="1">
+    <row r="3" spans="1:84" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -3616,15 +3961,15 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="5" spans="1:84">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
         <v>158</v>
-      </c>
-      <c r="B5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3632,11 +3977,6 @@
     <mergeCell ref="W2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3648,9 +3988,9 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>63</v>
       </c>
@@ -3667,7 +4007,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -3678,7 +4018,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -3703,10 +4043,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created Catch curve function based on Fish Forever Excel sheet
</commit_message>
<xml_diff>
--- a/Survey_DB.xlsx
+++ b/Survey_DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="25600" windowHeight="15720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wagner" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="Q9_Diana" sheetId="7" r:id="rId6"/>
     <sheet name="Ignacia" sheetId="8" r:id="rId7"/>
     <sheet name="Q9_Ignacia" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="184">
   <si>
     <t>ID_fisher</t>
   </si>
@@ -543,9 +544,6 @@
     <t>Gillnet sizes : 3-3.5 for shrimp/6 for corvina</t>
   </si>
   <si>
-    <t>5,6</t>
-  </si>
-  <si>
     <t>Hace 6 años eran mejores, gente respectaba y guara costa hacia su trabajo. Cambio y falta de recursos de guarda costa. Ademas narcotrafico</t>
   </si>
   <si>
@@ -568,6 +566,27 @@
   </si>
   <si>
     <t>conflicto grande de comunidades/no todos los asocidos pescan con cuerda o dentro del AMPR con esa arte de pesca/Muchos no-asociados pescan dentro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5/6</t>
+  </si>
+  <si>
+    <t>Q8.1</t>
+  </si>
+  <si>
+    <t>Q8.2</t>
+  </si>
+  <si>
+    <t>if they specified by gear</t>
+  </si>
+  <si>
+    <t>hours (avg)</t>
+  </si>
+  <si>
+    <t>trip_length_avgerage</t>
+  </si>
+  <si>
+    <t>trip_length_by_gear</t>
   </si>
 </sst>
 </file>
@@ -644,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -658,13 +677,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1210,17 +1230,17 @@
       <c r="V2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
       <c r="AO2" s="2" t="s">
         <v>46</v>
       </c>
@@ -1671,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG4"/>
+  <dimension ref="A1:CH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="BX4" sqref="BX4"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AR4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1721,41 +1741,986 @@
     <col min="43" max="43" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="10" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="10" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="7" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="10" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.1640625" customWidth="1"/>
+    <col min="47" max="47" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="7" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="7" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:86" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BR1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="BT1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="BV1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="BW1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="BY1" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="BZ1" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="CA1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="CC1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="CD1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="CE1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="CF1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="CH1" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:86" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="N2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="S2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BP2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="BQ2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="BR2" s="7"/>
+      <c r="BS2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BT2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="BX2" s="7"/>
+      <c r="BY2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="CC2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="CD2" s="7"/>
+      <c r="CE2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CF2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CG2" s="5"/>
+    </row>
+    <row r="3" spans="1:86" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="X3" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AA3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="AC3" s="10">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="10">
+        <v>6</v>
+      </c>
+      <c r="AE3" s="10">
+        <v>7</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS3" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AT3" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AU3" s="12"/>
+      <c r="AV3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AX3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="BD3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="BF3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="BJ3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="BK3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="BL3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="BM3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="BN3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="BO3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BP3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="BQ3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="BR3" s="10"/>
+      <c r="BS3" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT3" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="BU3" s="11"/>
+      <c r="BV3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="BW3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="BX3" s="10"/>
+      <c r="BY3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="BZ3" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="CA3" s="11"/>
+      <c r="CB3" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="CC3" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="CD3" s="10"/>
+      <c r="CE3" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF3" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="CG3" s="11"/>
+    </row>
+    <row r="4" spans="1:86" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="13">
+        <v>42567</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>164</v>
+      </c>
+      <c r="L4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M4">
+        <v>15</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>166</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>600</v>
+      </c>
+      <c r="V4" t="s">
+        <v>166</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>6</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <f>AVERAGE(500, 1000)</f>
+        <v>750</v>
+      </c>
+      <c r="AP4" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>12</v>
+      </c>
+      <c r="AV4">
+        <v>15</v>
+      </c>
+      <c r="AW4" s="15">
+        <f>AVERAGE(9,10,2)</f>
+        <v>7</v>
+      </c>
+      <c r="AX4" s="15">
+        <v>7</v>
+      </c>
+      <c r="AY4">
+        <f>AVERAGE(3000,4000)</f>
+        <v>3500</v>
+      </c>
+      <c r="BA4">
+        <f>AVERAGE(300000,400000)</f>
+        <v>350000</v>
+      </c>
+      <c r="BB4">
+        <v>2</v>
+      </c>
+      <c r="BC4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BD4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BE4">
+        <v>80000</v>
+      </c>
+      <c r="BF4" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="BG4">
+        <v>0.5</v>
+      </c>
+      <c r="BH4">
+        <v>0.5</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL4" s="16">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="16">
+        <v>1</v>
+      </c>
+      <c r="BN4" s="16">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP4" s="16">
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="16">
+        <v>1</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>171</v>
+      </c>
+      <c r="BS4">
+        <v>0</v>
+      </c>
+      <c r="BT4">
+        <v>1</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>175</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4">
+        <v>1</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>176</v>
+      </c>
+      <c r="BY4">
+        <v>1</v>
+      </c>
+      <c r="BZ4">
+        <v>1</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>172</v>
+      </c>
+      <c r="CB4">
+        <v>0</v>
+      </c>
+      <c r="CC4">
+        <v>1</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>173</v>
+      </c>
+      <c r="CE4">
+        <v>1</v>
+      </c>
+      <c r="CF4">
+        <v>0</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>174</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="W2:AE2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CF5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1937,11 +2902,8 @@
       <c r="CF1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="CG1" s="5" t="s">
-        <v>167</v>
-      </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1971,17 +2933,17 @@
       <c r="V2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
@@ -2106,7 +3068,7 @@
       </c>
       <c r="CF2" s="5"/>
     </row>
-    <row r="3" spans="1:85" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:84" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
@@ -2346,259 +3308,15 @@
       </c>
       <c r="CF3" s="11"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F4" s="14">
-        <v>42567</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>42</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>164</v>
-      </c>
-      <c r="L4" t="s">
-        <v>165</v>
-      </c>
-      <c r="M4">
-        <v>15</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="16">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>166</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>600</v>
-      </c>
-      <c r="V4" t="s">
-        <v>166</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>1</v>
-      </c>
-      <c r="Z4">
-        <v>1</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>1</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
-      <c r="AG4">
-        <v>1</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>6</v>
-      </c>
-      <c r="AJ4">
-        <v>1</v>
-      </c>
-      <c r="AK4">
-        <v>1</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>1</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
-        <f>AVERAGE(500, 1000)</f>
-        <v>750</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4">
-        <v>12</v>
-      </c>
-      <c r="AU4">
-        <v>15</v>
-      </c>
-      <c r="AV4" s="16">
-        <f>AVERAGE(9,10,2)</f>
-        <v>7</v>
-      </c>
-      <c r="AW4" s="16">
-        <v>7</v>
-      </c>
-      <c r="AX4">
-        <f>AVERAGE(3000,4000)</f>
-        <v>3500</v>
-      </c>
-      <c r="AZ4">
-        <f>AVERAGE(300000,400000)</f>
-        <v>350000</v>
-      </c>
-      <c r="BA4">
-        <v>2</v>
-      </c>
-      <c r="BB4" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="BC4" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="BD4">
-        <v>80000</v>
-      </c>
-      <c r="BE4" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="BF4">
-        <v>0.5</v>
-      </c>
-      <c r="BG4">
-        <v>0.5</v>
-      </c>
-      <c r="BH4">
-        <v>0</v>
-      </c>
-      <c r="BI4">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="BK4" s="17">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="17">
-        <v>1</v>
-      </c>
-      <c r="BM4" s="17">
-        <v>0</v>
-      </c>
-      <c r="BN4" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="BO4" s="17">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="17">
-        <v>1</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>172</v>
-      </c>
-      <c r="BR4">
-        <v>0</v>
-      </c>
-      <c r="BS4">
-        <v>1</v>
-      </c>
-      <c r="BT4" t="s">
-        <v>176</v>
-      </c>
-      <c r="BU4">
-        <v>0</v>
-      </c>
-      <c r="BV4">
-        <v>1</v>
-      </c>
-      <c r="BW4" t="s">
-        <v>177</v>
-      </c>
-      <c r="BX4">
-        <v>1</v>
-      </c>
-      <c r="BY4">
-        <v>1</v>
-      </c>
-      <c r="BZ4" t="s">
-        <v>173</v>
-      </c>
-      <c r="CA4">
-        <v>0</v>
-      </c>
-      <c r="CB4">
-        <v>1</v>
-      </c>
-      <c r="CC4" t="s">
-        <v>174</v>
-      </c>
-      <c r="CD4">
-        <v>1</v>
-      </c>
-      <c r="CE4">
-        <v>0</v>
-      </c>
-      <c r="CF4" t="s">
-        <v>175</v>
-      </c>
-      <c r="CG4" t="s">
-        <v>168</v>
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2609,12 +3327,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2670,25 +3388,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>159</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:84" x14ac:dyDescent="0.2">
       <c r="H1" s="2" t="s">
@@ -2903,700 +3616,17 @@
       <c r="V2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AU2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>30</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>114</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="BL2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>119</v>
-      </c>
-      <c r="BO2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="BP2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="BQ2" s="7"/>
-      <c r="BR2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BS2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BT2" s="5"/>
-      <c r="BU2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="BV2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="BW2" s="7"/>
-      <c r="BX2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BY2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="BZ2" s="5"/>
-      <c r="CA2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="CB2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="CC2" s="7"/>
-      <c r="CD2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="CE2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="CF2" s="5"/>
-    </row>
-    <row r="3" spans="1:84" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="W3" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="X3" s="10">
-        <v>2.75</v>
-      </c>
-      <c r="Y3" s="10">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="10">
-        <v>3.5</v>
-      </c>
-      <c r="AA3" s="10">
-        <v>4</v>
-      </c>
-      <c r="AB3" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="AC3" s="10">
-        <v>5</v>
-      </c>
-      <c r="AD3" s="10">
-        <v>6</v>
-      </c>
-      <c r="AE3" s="10">
-        <v>7</v>
-      </c>
-      <c r="AF3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV3" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AX3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY3" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="BB3" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="BC3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD3" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="BE3" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="BF3" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="BG3" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="BH3" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="BJ3" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="BK3" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="BL3" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="BM3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="BN3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="BO3" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="BP3" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="BQ3" s="10"/>
-      <c r="BR3" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="BS3" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BT3" s="11"/>
-      <c r="BU3" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="BV3" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="BW3" s="10"/>
-      <c r="BX3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="BY3" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="BZ3" s="11"/>
-      <c r="CA3" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="CB3" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="CC3" s="10"/>
-      <c r="CD3" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="CE3" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="CF3" s="11"/>
-    </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="W2:AE2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AT1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="BM1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BO1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="BQ1" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="BR1" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="BS1" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="BT1" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="BV1" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="BW1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="BX1" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="BY1" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="BZ1" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="CA1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="CB1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="CC1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="CD1" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="CE1" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="CF1" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="N2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3"/>
-      <c r="S2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
@@ -4044,4 +4074,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>